<commit_message>
Fixed some errors in the Gaussian weighted fits - more clean
</commit_message>
<xml_diff>
--- a/Data_Experimental_AJ/cellConditions_M.xlsx
+++ b/Data_Experimental_AJ/cellConditions_M.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>cellID</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>22-05-31_M7_P2_C3</t>
-  </si>
-  <si>
-    <t>shitty curve</t>
   </si>
   <si>
     <t>blebby only after activation</t>
@@ -465,7 +462,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,10 +599,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,24 +635,24 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -670,12 +664,12 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -687,12 +681,12 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -704,12 +698,12 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -721,12 +715,12 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>

</xml_diff>